<commit_message>
Commit for draft report materials
</commit_message>
<xml_diff>
--- a/DataDictionary.xlsx
+++ b/DataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rwildermuth\Dropbox\PhD_UMass\WA_QNM\WA_QNM_MSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC7E75F-D8D3-4406-B640-B0DAA983B9F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B89280-2BDE-46A4-9C26-FF8CADB32E7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41100" yWindow="2550" windowWidth="11025" windowHeight="9030" activeTab="2" xr2:uid="{3B0380DA-8E8E-491F-B6E9-18130E0320E1}"/>
+    <workbookView xWindow="9636" yWindow="4452" windowWidth="11028" windowHeight="7380" xr2:uid="{3B0380DA-8E8E-491F-B6E9-18130E0320E1}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
@@ -1323,25 +1323,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1659,7 +1659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A932C61-716A-419A-8DE2-BC8ADB6CDA34}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1764,7 +1764,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1902,19 +1902,19 @@
       <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="49" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="29" t="s">
@@ -1933,11 +1933,11 @@
       <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
       <c r="G3" t="s">
         <v>45</v>
       </c>
@@ -1955,11 +1955,11 @@
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
       <c r="G4" s="1" t="s">
         <v>32</v>
       </c>
@@ -1977,7 +1977,7 @@
       <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="49" t="s">
         <v>25</v>
       </c>
       <c r="C5" t="s">
@@ -2006,7 +2006,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="50"/>
+      <c r="B6" s="49"/>
       <c r="D6" s="24"/>
       <c r="G6" s="43" t="s">
         <v>293</v>
@@ -2025,19 +2025,19 @@
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="50" t="s">
         <v>293</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="D7" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="50" t="s">
+      <c r="E7" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="49" t="s">
         <v>30</v>
       </c>
       <c r="G7" s="29" t="s">
@@ -2058,11 +2058,11 @@
       <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="49"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
       <c r="G8" t="s">
         <v>32</v>
       </c>
@@ -2077,11 +2077,11 @@
       <c r="A9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="49"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
       <c r="G9" s="29" t="s">
         <v>140</v>
       </c>
@@ -2098,19 +2098,19 @@
       <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="49" t="s">
+      <c r="D10" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="50" t="s">
+      <c r="E10" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="50" t="s">
+      <c r="F10" s="49" t="s">
         <v>39</v>
       </c>
       <c r="G10" t="s">
@@ -2130,11 +2130,11 @@
       <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
       <c r="G11" s="29" t="s">
         <v>81</v>
       </c>
@@ -2153,11 +2153,11 @@
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
       <c r="G12" s="1" t="s">
         <v>296</v>
       </c>
@@ -2175,11 +2175,11 @@
       <c r="A13" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
       <c r="G13" s="16" t="s">
         <v>299</v>
       </c>
@@ -2191,7 +2191,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="50"/>
+      <c r="B14" s="49"/>
       <c r="D14" s="24"/>
       <c r="G14" s="43" t="s">
         <v>32</v>
@@ -2207,13 +2207,13 @@
       <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="49" t="s">
         <v>296</v>
       </c>
       <c r="C15" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="49" t="s">
+      <c r="D15" s="50" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="47" t="s">
@@ -2236,9 +2236,9 @@
       <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="50"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="47"/>
-      <c r="D16" s="49"/>
+      <c r="D16" s="50"/>
       <c r="E16" s="47"/>
       <c r="F16" s="47"/>
       <c r="G16" t="s">
@@ -2255,9 +2255,9 @@
       <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="50"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="47"/>
-      <c r="D17" s="49"/>
+      <c r="D17" s="50"/>
       <c r="E17" s="47"/>
       <c r="F17" s="47"/>
       <c r="G17" t="s">
@@ -2274,9 +2274,9 @@
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="50"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="47"/>
-      <c r="D18" s="49"/>
+      <c r="D18" s="50"/>
       <c r="E18" s="47"/>
       <c r="F18" s="47"/>
       <c r="G18" t="s">
@@ -2293,9 +2293,9 @@
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="50"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="47"/>
-      <c r="D19" s="49"/>
+      <c r="D19" s="50"/>
       <c r="E19" s="47"/>
       <c r="F19" s="47"/>
       <c r="G19" s="40" t="s">
@@ -2313,9 +2313,9 @@
       <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="50"/>
+      <c r="B20" s="49"/>
       <c r="C20" s="47"/>
-      <c r="D20" s="49"/>
+      <c r="D20" s="50"/>
       <c r="E20" s="47"/>
       <c r="F20" s="47"/>
       <c r="G20" s="41" t="s">
@@ -2333,9 +2333,9 @@
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="50"/>
+      <c r="B21" s="49"/>
       <c r="C21" s="47"/>
-      <c r="D21" s="49"/>
+      <c r="D21" s="50"/>
       <c r="E21" s="47"/>
       <c r="F21" s="47"/>
       <c r="G21" s="29" t="s">
@@ -2346,7 +2346,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="50"/>
+      <c r="B22" s="49"/>
       <c r="C22" s="33"/>
       <c r="D22" s="36"/>
       <c r="E22" s="33"/>
@@ -2362,7 +2362,7 @@
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="51" t="s">
         <v>299</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -2392,7 +2392,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="52"/>
+      <c r="B24" s="51"/>
       <c r="C24" s="28"/>
       <c r="D24" s="24"/>
       <c r="E24" s="23"/>
@@ -2405,7 +2405,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="52"/>
+      <c r="B25" s="51"/>
       <c r="C25" s="28"/>
       <c r="D25" s="24"/>
       <c r="E25" s="23"/>
@@ -2418,7 +2418,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="52"/>
+      <c r="B26" s="51"/>
       <c r="C26" s="28"/>
       <c r="D26" s="24"/>
       <c r="E26" s="23"/>
@@ -2466,7 +2466,7 @@
       <c r="A28" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="52" t="s">
+      <c r="B28" s="51" t="s">
         <v>59</v>
       </c>
       <c r="C28" t="s">
@@ -2495,7 +2495,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="52"/>
+      <c r="B29" s="51"/>
       <c r="D29" s="24"/>
       <c r="G29" s="27" t="s">
         <v>46</v>
@@ -2511,7 +2511,7 @@
       <c r="A30" t="s">
         <v>69</v>
       </c>
-      <c r="B30" s="52" t="s">
+      <c r="B30" s="51" t="s">
         <v>60</v>
       </c>
       <c r="C30" t="s">
@@ -2540,7 +2540,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="52"/>
+      <c r="B31" s="51"/>
       <c r="D31" s="24"/>
       <c r="G31" s="25" t="s">
         <v>61</v>
@@ -2553,7 +2553,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="52"/>
+      <c r="B32" s="51"/>
       <c r="D32" s="36"/>
       <c r="G32" s="38" t="s">
         <v>288</v>
@@ -2569,19 +2569,19 @@
       <c r="A33" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="52" t="s">
+      <c r="B33" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="50" t="s">
+      <c r="C33" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="D33" s="49" t="s">
+      <c r="D33" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="E33" s="50" t="s">
+      <c r="E33" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="50" t="s">
+      <c r="F33" s="49" t="s">
         <v>68</v>
       </c>
       <c r="G33" s="13" t="s">
@@ -2601,11 +2601,11 @@
       <c r="A34" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="52"/>
-      <c r="C34" s="50"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
       <c r="G34" s="13" t="s">
         <v>314</v>
       </c>
@@ -2620,19 +2620,19 @@
       <c r="A35" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="56" t="s">
+      <c r="B35" s="52" t="s">
         <v>314</v>
       </c>
-      <c r="C35" s="56" t="s">
+      <c r="C35" s="52" t="s">
         <v>291</v>
       </c>
-      <c r="D35" s="49" t="s">
+      <c r="D35" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="E35" s="55" t="s">
+      <c r="E35" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="F35" s="55" t="s">
+      <c r="F35" s="53" t="s">
         <v>260</v>
       </c>
       <c r="G35" s="13" t="s">
@@ -2652,11 +2652,11 @@
       <c r="A36" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="56"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
       <c r="G36" s="13" t="s">
         <v>145</v>
       </c>
@@ -2671,11 +2671,11 @@
       <c r="A37" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="56"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="55"/>
-      <c r="F37" s="55"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
       <c r="G37" s="41" t="s">
         <v>269</v>
       </c>
@@ -2691,7 +2691,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="56" t="s">
+      <c r="B38" s="52" t="s">
         <v>310</v>
       </c>
       <c r="C38" s="37" t="s">
@@ -2713,7 +2713,7 @@
       </c>
     </row>
     <row r="39" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="56"/>
+      <c r="B39" s="52"/>
       <c r="C39" s="37"/>
       <c r="D39" s="36"/>
       <c r="E39" s="35"/>
@@ -2749,16 +2749,16 @@
       <c r="A41" t="s">
         <v>70</v>
       </c>
-      <c r="B41" s="52" t="s">
+      <c r="B41" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="C41" s="52" t="s">
+      <c r="C41" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="D41" s="49" t="s">
+      <c r="D41" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="E41" s="50" t="s">
+      <c r="E41" s="49" t="s">
         <v>74</v>
       </c>
       <c r="G41" t="s">
@@ -2775,10 +2775,10 @@
       <c r="A42" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B42" s="52"/>
-      <c r="C42" s="52"/>
-      <c r="D42" s="49"/>
-      <c r="E42" s="50"/>
+      <c r="B42" s="51"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="49"/>
       <c r="G42" s="13" t="s">
         <v>145</v>
       </c>
@@ -2828,19 +2828,19 @@
       <c r="A44" t="s">
         <v>70</v>
       </c>
-      <c r="B44" s="50" t="s">
+      <c r="B44" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="50" t="s">
+      <c r="C44" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="D44" s="49" t="s">
+      <c r="D44" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="E44" s="50" t="s">
+      <c r="E44" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="F44" s="50" t="s">
+      <c r="F44" s="49" t="s">
         <v>78</v>
       </c>
       <c r="G44" s="18" t="s">
@@ -2860,11 +2860,11 @@
       <c r="A45" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B45" s="50"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="49"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="50"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="49"/>
+      <c r="F45" s="49"/>
       <c r="G45" s="44" t="s">
         <v>269</v>
       </c>
@@ -2883,11 +2883,11 @@
       <c r="A46" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="50"/>
-      <c r="C46" s="50"/>
-      <c r="D46" s="49"/>
-      <c r="E46" s="50"/>
-      <c r="F46" s="50"/>
+      <c r="B46" s="49"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="49"/>
       <c r="G46" s="18" t="s">
         <v>46</v>
       </c>
@@ -2902,11 +2902,11 @@
       <c r="A47" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B47" s="50"/>
-      <c r="C47" s="50"/>
-      <c r="D47" s="49"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="50"/>
+      <c r="B47" s="49"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="49"/>
       <c r="G47" s="18" t="s">
         <v>145</v>
       </c>
@@ -2921,11 +2921,11 @@
       <c r="A48" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B48" s="50"/>
-      <c r="C48" s="50"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="50"/>
+      <c r="B48" s="49"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="49"/>
       <c r="G48" s="44" t="s">
         <v>105</v>
       </c>
@@ -2941,10 +2941,10 @@
       <c r="A49" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B49" s="56" t="s">
+      <c r="B49" s="52" t="s">
         <v>270</v>
       </c>
-      <c r="C49" s="50" t="s">
+      <c r="C49" s="49" t="s">
         <v>313</v>
       </c>
       <c r="D49" s="12"/>
@@ -2968,8 +2968,8 @@
       <c r="A50" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B50" s="56"/>
-      <c r="C50" s="50"/>
+      <c r="B50" s="52"/>
+      <c r="C50" s="49"/>
       <c r="D50" s="12"/>
       <c r="G50" s="41" t="s">
         <v>45</v>
@@ -2991,8 +2991,8 @@
       <c r="A51" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B51" s="56"/>
-      <c r="C51" s="50"/>
+      <c r="B51" s="52"/>
+      <c r="C51" s="49"/>
       <c r="D51" s="12"/>
       <c r="G51" s="10" t="s">
         <v>145</v>
@@ -3005,7 +3005,7 @@
       </c>
     </row>
     <row r="52" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="56"/>
+      <c r="B52" s="52"/>
       <c r="D52" s="24"/>
       <c r="G52" s="25" t="s">
         <v>314</v>
@@ -3021,19 +3021,19 @@
       <c r="A53" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B53" s="53" t="s">
+      <c r="B53" s="54" t="s">
         <v>297</v>
       </c>
-      <c r="C53" s="53" t="s">
+      <c r="C53" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="D53" s="54" t="s">
+      <c r="D53" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="E53" s="53" t="s">
+      <c r="E53" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="F53" s="53" t="s">
+      <c r="F53" s="54" t="s">
         <v>95</v>
       </c>
       <c r="G53" s="29" t="s">
@@ -3053,11 +3053,11 @@
       <c r="A54" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B54" s="53"/>
-      <c r="C54" s="53"/>
-      <c r="D54" s="54"/>
-      <c r="E54" s="53"/>
-      <c r="F54" s="53"/>
+      <c r="B54" s="54"/>
+      <c r="C54" s="54"/>
+      <c r="D54" s="55"/>
+      <c r="E54" s="54"/>
+      <c r="F54" s="54"/>
       <c r="G54" s="29" t="s">
         <v>89</v>
       </c>
@@ -3075,16 +3075,16 @@
       <c r="A55" t="s">
         <v>85</v>
       </c>
-      <c r="B55" s="50" t="s">
+      <c r="B55" s="49" t="s">
         <v>298</v>
       </c>
-      <c r="C55" s="50" t="s">
+      <c r="C55" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="D55" s="49" t="s">
+      <c r="D55" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="F55" s="50" t="s">
+      <c r="F55" s="49" t="s">
         <v>93</v>
       </c>
       <c r="G55" t="s">
@@ -3104,10 +3104,10 @@
       <c r="A56" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B56" s="50"/>
-      <c r="C56" s="50"/>
-      <c r="D56" s="49"/>
-      <c r="F56" s="50"/>
+      <c r="B56" s="49"/>
+      <c r="C56" s="49"/>
+      <c r="D56" s="50"/>
+      <c r="F56" s="49"/>
       <c r="G56" s="29" t="s">
         <v>140</v>
       </c>
@@ -3124,7 +3124,7 @@
       <c r="A57" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="B57" s="50"/>
+      <c r="B57" s="49"/>
       <c r="D57" s="24"/>
       <c r="G57" s="27" t="s">
         <v>61</v>
@@ -3142,7 +3142,7 @@
       <c r="A58" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="B58" s="50"/>
+      <c r="B58" s="49"/>
       <c r="D58" s="24"/>
       <c r="G58" s="27" t="s">
         <v>45</v>
@@ -3160,7 +3160,7 @@
       <c r="A59" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="B59" s="50"/>
+      <c r="B59" s="49"/>
       <c r="D59" s="24"/>
       <c r="G59" s="34" t="s">
         <v>296</v>
@@ -3178,19 +3178,19 @@
       <c r="A60" t="s">
         <v>85</v>
       </c>
-      <c r="B60" s="50" t="s">
+      <c r="B60" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="C60" s="50" t="s">
+      <c r="C60" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="D60" s="49" t="s">
+      <c r="D60" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="E60" s="50" t="s">
+      <c r="E60" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="F60" s="50" t="s">
+      <c r="F60" s="49" t="s">
         <v>196</v>
       </c>
       <c r="G60" s="41" t="s">
@@ -3210,11 +3210,11 @@
       <c r="A61" t="s">
         <v>85</v>
       </c>
-      <c r="B61" s="50"/>
-      <c r="C61" s="50"/>
-      <c r="D61" s="49"/>
-      <c r="E61" s="50"/>
-      <c r="F61" s="50"/>
+      <c r="B61" s="49"/>
+      <c r="C61" s="49"/>
+      <c r="D61" s="50"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="49"/>
       <c r="G61" t="s">
         <v>270</v>
       </c>
@@ -3229,11 +3229,11 @@
       <c r="A62" t="s">
         <v>85</v>
       </c>
-      <c r="B62" s="50"/>
-      <c r="C62" s="50"/>
-      <c r="D62" s="49"/>
-      <c r="E62" s="50"/>
-      <c r="F62" s="50"/>
+      <c r="B62" s="49"/>
+      <c r="C62" s="49"/>
+      <c r="D62" s="50"/>
+      <c r="E62" s="49"/>
+      <c r="F62" s="49"/>
       <c r="G62" s="29" t="s">
         <v>105</v>
       </c>
@@ -3249,11 +3249,11 @@
       <c r="A63" t="s">
         <v>85</v>
       </c>
-      <c r="B63" s="50"/>
-      <c r="C63" s="50"/>
-      <c r="D63" s="49"/>
-      <c r="E63" s="50"/>
-      <c r="F63" s="50"/>
+      <c r="B63" s="49"/>
+      <c r="C63" s="49"/>
+      <c r="D63" s="50"/>
+      <c r="E63" s="49"/>
+      <c r="F63" s="49"/>
       <c r="G63" s="27" t="s">
         <v>314</v>
       </c>
@@ -3268,11 +3268,11 @@
       <c r="A64" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B64" s="50"/>
-      <c r="C64" s="50"/>
-      <c r="D64" s="49"/>
-      <c r="E64" s="50"/>
-      <c r="F64" s="50"/>
+      <c r="B64" s="49"/>
+      <c r="C64" s="49"/>
+      <c r="D64" s="50"/>
+      <c r="E64" s="49"/>
+      <c r="F64" s="49"/>
       <c r="G64" s="29" t="s">
         <v>267</v>
       </c>
@@ -3283,7 +3283,7 @@
       </c>
     </row>
     <row r="65" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="50"/>
+      <c r="B65" s="49"/>
       <c r="D65" s="24"/>
       <c r="G65" s="25" t="s">
         <v>298</v>
@@ -3296,7 +3296,7 @@
       </c>
     </row>
     <row r="66" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="50"/>
+      <c r="B66" s="49"/>
       <c r="D66" s="24"/>
       <c r="G66" s="41" t="s">
         <v>44</v>
@@ -3306,7 +3306,7 @@
       </c>
     </row>
     <row r="67" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="50"/>
+      <c r="B67" s="49"/>
       <c r="D67" s="24"/>
       <c r="G67" s="41" t="s">
         <v>46</v>
@@ -3321,7 +3321,7 @@
       </c>
     </row>
     <row r="68" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="50"/>
+      <c r="B68" s="49"/>
       <c r="D68" s="36"/>
       <c r="G68" s="38" t="s">
         <v>315</v>
@@ -3337,7 +3337,7 @@
       </c>
     </row>
     <row r="69" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="50"/>
+      <c r="B69" s="49"/>
       <c r="D69" s="36"/>
       <c r="G69" s="38" t="s">
         <v>288</v>
@@ -3353,19 +3353,19 @@
       <c r="A70" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="B70" s="53" t="s">
+      <c r="B70" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="C70" s="53" t="s">
+      <c r="C70" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="D70" s="54" t="s">
+      <c r="D70" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="E70" s="53" t="s">
+      <c r="E70" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="F70" s="53" t="s">
+      <c r="F70" s="54" t="s">
         <v>167</v>
       </c>
       <c r="G70" s="41" t="s">
@@ -3385,11 +3385,11 @@
       <c r="A71" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="B71" s="53"/>
-      <c r="C71" s="53"/>
-      <c r="D71" s="54"/>
-      <c r="E71" s="53"/>
-      <c r="F71" s="53"/>
+      <c r="B71" s="54"/>
+      <c r="C71" s="54"/>
+      <c r="D71" s="55"/>
+      <c r="E71" s="54"/>
+      <c r="F71" s="54"/>
       <c r="G71" s="41" t="s">
         <v>268</v>
       </c>
@@ -3407,11 +3407,11 @@
       <c r="A72" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="B72" s="53"/>
-      <c r="C72" s="53"/>
-      <c r="D72" s="54"/>
-      <c r="E72" s="53"/>
-      <c r="F72" s="53"/>
+      <c r="B72" s="54"/>
+      <c r="C72" s="54"/>
+      <c r="D72" s="55"/>
+      <c r="E72" s="54"/>
+      <c r="F72" s="54"/>
       <c r="G72" s="41" t="s">
         <v>269</v>
       </c>
@@ -3426,11 +3426,11 @@
       <c r="A73" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="B73" s="53"/>
-      <c r="C73" s="53"/>
-      <c r="D73" s="54"/>
-      <c r="E73" s="53"/>
-      <c r="F73" s="53"/>
+      <c r="B73" s="54"/>
+      <c r="C73" s="54"/>
+      <c r="D73" s="55"/>
+      <c r="E73" s="54"/>
+      <c r="F73" s="54"/>
       <c r="G73" s="41" t="s">
         <v>105</v>
       </c>
@@ -3445,11 +3445,11 @@
       <c r="A74" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="B74" s="53"/>
-      <c r="C74" s="53"/>
-      <c r="D74" s="54"/>
-      <c r="E74" s="53"/>
-      <c r="F74" s="53"/>
+      <c r="B74" s="54"/>
+      <c r="C74" s="54"/>
+      <c r="D74" s="55"/>
+      <c r="E74" s="54"/>
+      <c r="F74" s="54"/>
       <c r="G74" s="41" t="s">
         <v>45</v>
       </c>
@@ -3467,11 +3467,11 @@
       <c r="A75" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="B75" s="53"/>
-      <c r="C75" s="53"/>
-      <c r="D75" s="54"/>
-      <c r="E75" s="53"/>
-      <c r="F75" s="53"/>
+      <c r="B75" s="54"/>
+      <c r="C75" s="54"/>
+      <c r="D75" s="55"/>
+      <c r="E75" s="54"/>
+      <c r="F75" s="54"/>
       <c r="G75" s="41" t="s">
         <v>288</v>
       </c>
@@ -3486,16 +3486,16 @@
       <c r="A76" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="B76" s="53" t="s">
+      <c r="B76" s="54" t="s">
         <v>303</v>
       </c>
-      <c r="C76" s="53" t="s">
+      <c r="C76" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="D76" s="54" t="s">
+      <c r="D76" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="F76" s="53" t="s">
+      <c r="F76" s="54" t="s">
         <v>12</v>
       </c>
       <c r="G76" s="41" t="s">
@@ -3512,10 +3512,10 @@
       <c r="A77" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="B77" s="53"/>
-      <c r="C77" s="53"/>
-      <c r="D77" s="54"/>
-      <c r="F77" s="53"/>
+      <c r="B77" s="54"/>
+      <c r="C77" s="54"/>
+      <c r="D77" s="55"/>
+      <c r="F77" s="54"/>
       <c r="G77" s="41" t="s">
         <v>46</v>
       </c>
@@ -3533,10 +3533,10 @@
       <c r="A78" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="B78" s="53"/>
-      <c r="C78" s="53"/>
-      <c r="D78" s="54"/>
-      <c r="F78" s="53"/>
+      <c r="B78" s="54"/>
+      <c r="C78" s="54"/>
+      <c r="D78" s="55"/>
+      <c r="F78" s="54"/>
       <c r="G78" s="41" t="s">
         <v>267</v>
       </c>
@@ -3566,7 +3566,7 @@
       <c r="A80" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="B80" s="56" t="s">
+      <c r="B80" s="52" t="s">
         <v>315</v>
       </c>
       <c r="C80" s="34" t="s">
@@ -3598,7 +3598,7 @@
       <c r="A81" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="B81" s="56"/>
+      <c r="B81" s="52"/>
       <c r="D81" s="45"/>
       <c r="G81" s="34" t="s">
         <v>314</v>
@@ -3617,7 +3617,7 @@
       <c r="A82" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="B82" s="56"/>
+      <c r="B82" s="52"/>
       <c r="D82" s="45"/>
       <c r="G82" s="34" t="s">
         <v>269</v>
@@ -3633,7 +3633,7 @@
       <c r="A83" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="B83" s="56"/>
+      <c r="B83" s="52"/>
       <c r="D83" s="45"/>
       <c r="G83" s="34" t="s">
         <v>45</v>
@@ -3652,7 +3652,7 @@
       <c r="A84" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="B84" s="56"/>
+      <c r="B84" s="52"/>
       <c r="D84" s="45"/>
       <c r="G84" s="34" t="s">
         <v>288</v>
@@ -3729,19 +3729,19 @@
       <c r="A88" t="s">
         <v>155</v>
       </c>
-      <c r="B88" s="49" t="s">
+      <c r="B88" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="C88" s="50" t="s">
+      <c r="C88" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="D88" s="49" t="s">
+      <c r="D88" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="E88" s="50" t="s">
+      <c r="E88" s="49" t="s">
         <v>154</v>
       </c>
-      <c r="F88" s="50" t="s">
+      <c r="F88" s="49" t="s">
         <v>153</v>
       </c>
       <c r="G88" s="29" t="s">
@@ -3762,11 +3762,11 @@
       <c r="A89" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B89" s="49"/>
-      <c r="C89" s="50"/>
-      <c r="D89" s="49"/>
-      <c r="E89" s="50"/>
-      <c r="F89" s="50"/>
+      <c r="B89" s="50"/>
+      <c r="C89" s="49"/>
+      <c r="D89" s="50"/>
+      <c r="E89" s="49"/>
+      <c r="F89" s="49"/>
       <c r="G89" s="29" t="s">
         <v>44</v>
       </c>
@@ -3787,11 +3787,11 @@
       <c r="A90" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B90" s="49"/>
-      <c r="C90" s="50"/>
-      <c r="D90" s="49"/>
-      <c r="E90" s="50"/>
-      <c r="F90" s="50"/>
+      <c r="B90" s="50"/>
+      <c r="C90" s="49"/>
+      <c r="D90" s="50"/>
+      <c r="E90" s="49"/>
+      <c r="F90" s="49"/>
       <c r="G90" s="29" t="s">
         <v>110</v>
       </c>
@@ -3810,11 +3810,11 @@
       <c r="A91" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B91" s="49"/>
-      <c r="C91" s="50"/>
-      <c r="D91" s="49"/>
-      <c r="E91" s="50"/>
-      <c r="F91" s="50"/>
+      <c r="B91" s="50"/>
+      <c r="C91" s="49"/>
+      <c r="D91" s="50"/>
+      <c r="E91" s="49"/>
+      <c r="F91" s="49"/>
       <c r="G91" s="29" t="s">
         <v>61</v>
       </c>
@@ -3833,11 +3833,11 @@
       <c r="A92" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B92" s="49"/>
-      <c r="C92" s="50"/>
-      <c r="D92" s="49"/>
-      <c r="E92" s="50"/>
-      <c r="F92" s="50"/>
+      <c r="B92" s="50"/>
+      <c r="C92" s="49"/>
+      <c r="D92" s="50"/>
+      <c r="E92" s="49"/>
+      <c r="F92" s="49"/>
       <c r="G92" s="6" t="s">
         <v>314</v>
       </c>
@@ -3852,11 +3852,11 @@
       <c r="A93" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B93" s="49"/>
-      <c r="C93" s="50"/>
-      <c r="D93" s="49"/>
-      <c r="E93" s="50"/>
-      <c r="F93" s="50"/>
+      <c r="B93" s="50"/>
+      <c r="C93" s="49"/>
+      <c r="D93" s="50"/>
+      <c r="E93" s="49"/>
+      <c r="F93" s="49"/>
       <c r="G93" s="6" t="s">
         <v>46</v>
       </c>
@@ -3871,11 +3871,11 @@
       <c r="A94" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B94" s="49"/>
-      <c r="C94" s="50"/>
-      <c r="D94" s="49"/>
-      <c r="E94" s="50"/>
-      <c r="F94" s="50"/>
+      <c r="B94" s="50"/>
+      <c r="C94" s="49"/>
+      <c r="D94" s="50"/>
+      <c r="E94" s="49"/>
+      <c r="F94" s="49"/>
       <c r="G94" s="6" t="s">
         <v>45</v>
       </c>
@@ -3890,11 +3890,11 @@
       <c r="A95" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B95" s="49"/>
-      <c r="C95" s="50"/>
-      <c r="D95" s="49"/>
-      <c r="E95" s="50"/>
-      <c r="F95" s="50"/>
+      <c r="B95" s="50"/>
+      <c r="C95" s="49"/>
+      <c r="D95" s="50"/>
+      <c r="E95" s="49"/>
+      <c r="F95" s="49"/>
       <c r="G95" s="13" t="s">
         <v>269</v>
       </c>
@@ -3903,7 +3903,7 @@
       </c>
     </row>
     <row r="96" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="49"/>
+      <c r="B96" s="50"/>
       <c r="D96" s="24"/>
       <c r="G96" s="27" t="s">
         <v>60</v>
@@ -3916,7 +3916,7 @@
       </c>
     </row>
     <row r="97" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="49"/>
+      <c r="B97" s="50"/>
       <c r="D97" s="36"/>
       <c r="G97" s="34" t="s">
         <v>310</v>
@@ -3991,59 +3991,6 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="B15:B22"/>
-    <mergeCell ref="B88:B97"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="B60:B69"/>
-    <mergeCell ref="B80:B84"/>
-    <mergeCell ref="B55:B59"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="F44:F48"/>
-    <mergeCell ref="E44:E48"/>
-    <mergeCell ref="D44:D48"/>
-    <mergeCell ref="C44:C48"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="C60:C64"/>
-    <mergeCell ref="D60:D64"/>
-    <mergeCell ref="E60:E64"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C15:C21"/>
-    <mergeCell ref="D15:D21"/>
-    <mergeCell ref="E15:E21"/>
-    <mergeCell ref="F15:F21"/>
-    <mergeCell ref="F60:F64"/>
     <mergeCell ref="F88:F95"/>
     <mergeCell ref="E88:E95"/>
     <mergeCell ref="D88:D95"/>
@@ -4052,6 +3999,14 @@
     <mergeCell ref="D70:D75"/>
     <mergeCell ref="E70:E75"/>
     <mergeCell ref="F70:F75"/>
+    <mergeCell ref="C76:C78"/>
+    <mergeCell ref="D76:D78"/>
+    <mergeCell ref="F76:F78"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C15:C21"/>
+    <mergeCell ref="D15:D21"/>
+    <mergeCell ref="E15:E21"/>
+    <mergeCell ref="F15:F21"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="D7:D9"/>
@@ -4061,10 +4016,55 @@
     <mergeCell ref="D10:D13"/>
     <mergeCell ref="E10:E13"/>
     <mergeCell ref="F10:F13"/>
+    <mergeCell ref="C60:C64"/>
+    <mergeCell ref="D60:D64"/>
+    <mergeCell ref="E60:E64"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="F60:F64"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="F44:F48"/>
+    <mergeCell ref="E44:E48"/>
+    <mergeCell ref="D44:D48"/>
+    <mergeCell ref="C44:C48"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B15:B22"/>
+    <mergeCell ref="B88:B97"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B60:B69"/>
+    <mergeCell ref="B80:B84"/>
+    <mergeCell ref="B55:B59"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="B53:B54"/>
     <mergeCell ref="B76:B78"/>
-    <mergeCell ref="C76:C78"/>
-    <mergeCell ref="D76:D78"/>
-    <mergeCell ref="F76:F78"/>
     <mergeCell ref="B70:B75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4076,7 +4076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FE08BE0-37AB-49B7-9C5B-E7B942F7E8DC}">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J46" sqref="J46"/>
     </sheetView>
@@ -4130,19 +4130,19 @@
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="49" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="56" t="s">
         <v>170</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="49" t="s">
         <v>171</v>
       </c>
       <c r="G2" t="s">
@@ -4162,11 +4162,11 @@
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="50"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="49"/>
       <c r="G3" s="27" t="s">
         <v>32</v>
       </c>
@@ -4216,19 +4216,19 @@
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="50" t="s">
         <v>293</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="50" t="s">
+      <c r="E5" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="50" t="s">
+      <c r="F5" s="49" t="s">
         <v>30</v>
       </c>
       <c r="G5" s="29" t="s">
@@ -4249,11 +4249,11 @@
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
       <c r="G6" t="s">
         <v>32</v>
       </c>
@@ -4268,7 +4268,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="49"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="26"/>
       <c r="D7" s="24"/>
       <c r="G7" s="25" t="s">
@@ -4285,7 +4285,7 @@
       <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="53" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -4315,7 +4315,7 @@
       <c r="K8" s="29"/>
     </row>
     <row r="9" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="55"/>
+      <c r="B9" s="53"/>
       <c r="C9" s="28"/>
       <c r="D9" s="24"/>
       <c r="E9" s="28"/>
@@ -4331,7 +4331,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="55"/>
+      <c r="B10" s="53"/>
       <c r="C10" s="28"/>
       <c r="D10" s="24"/>
       <c r="E10" s="28"/>
@@ -4347,7 +4347,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="55"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="28"/>
       <c r="D11" s="24"/>
       <c r="E11" s="28"/>
@@ -4398,7 +4398,7 @@
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="49" t="s">
         <v>172</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -4427,7 +4427,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="50"/>
+      <c r="B14" s="49"/>
       <c r="D14" s="24"/>
       <c r="G14" s="25" t="s">
         <v>233</v>
@@ -4443,7 +4443,7 @@
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="49" t="s">
         <v>304</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -4469,7 +4469,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="50"/>
+      <c r="B16" s="49"/>
       <c r="D16" s="24"/>
       <c r="E16" s="26"/>
       <c r="G16" s="25" t="s">
@@ -4486,7 +4486,7 @@
       <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="51" t="s">
         <v>296</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -4512,7 +4512,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="52"/>
+      <c r="B18" s="51"/>
       <c r="D18" s="24"/>
       <c r="E18" s="26"/>
       <c r="G18" s="27" t="s">
@@ -4526,7 +4526,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="52"/>
+      <c r="B19" s="51"/>
       <c r="D19" s="24"/>
       <c r="E19" s="26"/>
       <c r="G19" s="27" t="s">
@@ -4540,7 +4540,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="52"/>
+      <c r="B20" s="51"/>
       <c r="D20" s="24"/>
       <c r="E20" s="26"/>
       <c r="G20" s="27" t="s">
@@ -4557,7 +4557,7 @@
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="51" t="s">
         <v>299</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -4587,7 +4587,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="52"/>
+      <c r="B22" s="51"/>
       <c r="C22" s="28"/>
       <c r="D22" s="24"/>
       <c r="E22" s="23"/>
@@ -4606,19 +4606,19 @@
       <c r="A23" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="50" t="s">
         <v>175</v>
       </c>
-      <c r="C23" s="50" t="s">
+      <c r="C23" s="49" t="s">
         <v>182</v>
       </c>
-      <c r="D23" s="49" t="s">
+      <c r="D23" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="E23" s="51" t="s">
+      <c r="E23" s="56" t="s">
         <v>184</v>
       </c>
-      <c r="F23" s="50" t="s">
+      <c r="F23" s="49" t="s">
         <v>12</v>
       </c>
       <c r="G23" s="9" t="s">
@@ -4633,11 +4633,11 @@
       <c r="A24" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="49"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="50"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="49"/>
       <c r="G24" s="19" t="s">
         <v>205</v>
       </c>
@@ -4655,11 +4655,11 @@
       <c r="A25" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="49"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="50"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="49"/>
       <c r="G25" s="5" t="s">
         <v>201</v>
       </c>
@@ -4677,11 +4677,11 @@
       <c r="A26" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="49"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="50"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="49"/>
       <c r="G26" s="5" t="s">
         <v>298</v>
       </c>
@@ -4696,11 +4696,11 @@
       <c r="A27" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="49"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="50"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="49"/>
       <c r="G27" s="5" t="s">
         <v>198</v>
       </c>
@@ -4715,11 +4715,11 @@
       <c r="A28" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="49"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="50"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="49"/>
       <c r="G28" s="10" t="s">
         <v>261</v>
       </c>
@@ -4734,11 +4734,11 @@
       <c r="A29" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="49"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="50"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="49"/>
       <c r="G29" s="10" t="s">
         <v>231</v>
       </c>
@@ -4753,11 +4753,11 @@
       <c r="A30" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B30" s="49"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="50"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="49"/>
       <c r="G30" s="10" t="s">
         <v>266</v>
       </c>
@@ -4769,7 +4769,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="49"/>
+      <c r="B31" s="50"/>
       <c r="D31" s="24"/>
       <c r="E31" s="26"/>
       <c r="G31" s="25" t="s">
@@ -4783,7 +4783,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="49"/>
+      <c r="B32" s="50"/>
       <c r="D32" s="24"/>
       <c r="E32" s="26"/>
       <c r="G32" s="25" t="s">
@@ -4800,7 +4800,7 @@
       <c r="A33" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="52" t="s">
+      <c r="B33" s="51" t="s">
         <v>233</v>
       </c>
       <c r="D33" s="12"/>
@@ -4819,7 +4819,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="52"/>
+      <c r="B34" s="51"/>
       <c r="D34" s="24"/>
       <c r="E34" s="26"/>
       <c r="G34" s="27" t="s">
@@ -4837,7 +4837,7 @@
       <c r="A35" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="50" t="s">
+      <c r="B35" s="49" t="s">
         <v>188</v>
       </c>
       <c r="C35" s="5" t="s">
@@ -4860,7 +4860,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="50"/>
+      <c r="B36" s="49"/>
       <c r="D36" s="24"/>
       <c r="E36" s="26"/>
       <c r="G36" s="27" t="s">
@@ -4877,19 +4877,19 @@
       <c r="A37" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="50" t="s">
+      <c r="B37" s="49" t="s">
         <v>262</v>
       </c>
-      <c r="C37" s="50" t="s">
+      <c r="C37" s="49" t="s">
         <v>192</v>
       </c>
-      <c r="D37" s="49" t="s">
+      <c r="D37" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="E37" s="51" t="s">
+      <c r="E37" s="56" t="s">
         <v>193</v>
       </c>
-      <c r="F37" s="50" t="s">
+      <c r="F37" s="49" t="s">
         <v>12</v>
       </c>
       <c r="G37" s="13" t="s">
@@ -4909,11 +4909,11 @@
       <c r="A38" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="50"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="51"/>
-      <c r="F38" s="50"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="49"/>
       <c r="G38" s="17" t="s">
         <v>190</v>
       </c>
@@ -4948,7 +4948,7 @@
       <c r="A40" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B40" s="49" t="s">
+      <c r="B40" s="50" t="s">
         <v>297</v>
       </c>
       <c r="C40" s="8" t="s">
@@ -4980,7 +4980,7 @@
       </c>
     </row>
     <row r="41" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="49"/>
+      <c r="B41" s="50"/>
       <c r="C41" s="28"/>
       <c r="D41" s="24"/>
       <c r="E41" s="28"/>
@@ -4996,7 +4996,7 @@
       </c>
     </row>
     <row r="42" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="49"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="28"/>
       <c r="D42" s="24"/>
       <c r="E42" s="28"/>
@@ -5012,7 +5012,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="49"/>
+      <c r="B43" s="50"/>
       <c r="C43" s="28"/>
       <c r="D43" s="24"/>
       <c r="E43" s="28"/>
@@ -5031,19 +5031,19 @@
       <c r="A44" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="55" t="s">
+      <c r="B44" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="55" t="s">
+      <c r="C44" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="D44" s="49" t="s">
+      <c r="D44" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="E44" s="55" t="s">
+      <c r="E44" s="53" t="s">
         <v>197</v>
       </c>
-      <c r="F44" s="55" t="s">
+      <c r="F44" s="53" t="s">
         <v>196</v>
       </c>
       <c r="G44" t="s">
@@ -5060,11 +5060,11 @@
       <c r="A45" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="55"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="49"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
+      <c r="B45" s="53"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
       <c r="G45" t="s">
         <v>266</v>
       </c>
@@ -5079,11 +5079,11 @@
       <c r="A46" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B46" s="55"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="49"/>
-      <c r="E46" s="55"/>
-      <c r="F46" s="55"/>
+      <c r="B46" s="53"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="53"/>
+      <c r="F46" s="53"/>
       <c r="G46" t="s">
         <v>229</v>
       </c>
@@ -5127,19 +5127,19 @@
       <c r="A49" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B49" s="50" t="s">
+      <c r="B49" s="49" t="s">
         <v>198</v>
       </c>
-      <c r="C49" s="50" t="s">
+      <c r="C49" s="49" t="s">
         <v>199</v>
       </c>
-      <c r="D49" s="49" t="s">
+      <c r="D49" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="E49" s="51" t="s">
+      <c r="E49" s="56" t="s">
         <v>204</v>
       </c>
-      <c r="F49" s="50" t="s">
+      <c r="F49" s="49" t="s">
         <v>200</v>
       </c>
       <c r="G49" t="s">
@@ -5159,11 +5159,11 @@
       <c r="A50" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B50" s="50"/>
-      <c r="C50" s="50"/>
-      <c r="D50" s="49"/>
-      <c r="E50" s="51"/>
-      <c r="F50" s="50"/>
+      <c r="B50" s="49"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="56"/>
+      <c r="F50" s="49"/>
       <c r="G50" s="19" t="s">
         <v>205</v>
       </c>
@@ -5181,11 +5181,11 @@
       <c r="A51" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B51" s="50"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="49"/>
-      <c r="E51" s="51"/>
-      <c r="F51" s="50"/>
+      <c r="B51" s="49"/>
+      <c r="C51" s="49"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="56"/>
+      <c r="F51" s="49"/>
       <c r="G51" s="5" t="s">
         <v>201</v>
       </c>
@@ -5200,11 +5200,11 @@
       <c r="A52" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B52" s="50"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="49"/>
-      <c r="E52" s="51"/>
-      <c r="F52" s="50"/>
+      <c r="B52" s="49"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="56"/>
+      <c r="F52" s="49"/>
       <c r="G52" s="10" t="s">
         <v>249</v>
       </c>
@@ -5219,11 +5219,11 @@
       <c r="A53" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B53" s="50"/>
-      <c r="C53" s="50"/>
-      <c r="D53" s="49"/>
-      <c r="E53" s="51"/>
-      <c r="F53" s="50"/>
+      <c r="B53" s="49"/>
+      <c r="C53" s="49"/>
+      <c r="D53" s="50"/>
+      <c r="E53" s="56"/>
+      <c r="F53" s="49"/>
       <c r="G53" s="29" t="s">
         <v>190</v>
       </c>
@@ -5242,19 +5242,19 @@
       <c r="A54" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B54" s="50" t="s">
+      <c r="B54" s="49" t="s">
         <v>201</v>
       </c>
-      <c r="C54" s="50" t="s">
+      <c r="C54" s="49" t="s">
         <v>218</v>
       </c>
-      <c r="D54" s="49" t="s">
+      <c r="D54" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="E54" s="51" t="s">
+      <c r="E54" s="56" t="s">
         <v>220</v>
       </c>
-      <c r="F54" s="50" t="s">
+      <c r="F54" s="49" t="s">
         <v>219</v>
       </c>
       <c r="G54" t="s">
@@ -5274,11 +5274,11 @@
       <c r="A55" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B55" s="50"/>
-      <c r="C55" s="50"/>
-      <c r="D55" s="49"/>
-      <c r="E55" s="51"/>
-      <c r="F55" s="50"/>
+      <c r="B55" s="49"/>
+      <c r="C55" s="49"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="56"/>
+      <c r="F55" s="49"/>
       <c r="G55" s="19" t="s">
         <v>205</v>
       </c>
@@ -5296,11 +5296,11 @@
       <c r="A56" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B56" s="50"/>
-      <c r="C56" s="50"/>
-      <c r="D56" s="49"/>
-      <c r="E56" s="51"/>
-      <c r="F56" s="50"/>
+      <c r="B56" s="49"/>
+      <c r="C56" s="49"/>
+      <c r="D56" s="50"/>
+      <c r="E56" s="56"/>
+      <c r="F56" s="49"/>
       <c r="G56" s="10" t="s">
         <v>231</v>
       </c>
@@ -5315,11 +5315,11 @@
       <c r="A57" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B57" s="50"/>
-      <c r="C57" s="50"/>
-      <c r="D57" s="49"/>
-      <c r="E57" s="51"/>
-      <c r="F57" s="50"/>
+      <c r="B57" s="49"/>
+      <c r="C57" s="49"/>
+      <c r="D57" s="50"/>
+      <c r="E57" s="56"/>
+      <c r="F57" s="49"/>
       <c r="G57" s="10" t="s">
         <v>249</v>
       </c>
@@ -5334,19 +5334,19 @@
       <c r="A58" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B58" s="53" t="s">
+      <c r="B58" s="54" t="s">
         <v>205</v>
       </c>
-      <c r="C58" s="53" t="s">
+      <c r="C58" s="54" t="s">
         <v>209</v>
       </c>
-      <c r="D58" s="54" t="s">
+      <c r="D58" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="E58" s="57" t="s">
+      <c r="E58" s="58" t="s">
         <v>204</v>
       </c>
-      <c r="F58" s="53" t="s">
+      <c r="F58" s="54" t="s">
         <v>12</v>
       </c>
       <c r="G58" s="19" t="s">
@@ -5369,11 +5369,11 @@
       <c r="A59" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B59" s="53"/>
-      <c r="C59" s="53"/>
-      <c r="D59" s="54"/>
-      <c r="E59" s="57"/>
-      <c r="F59" s="53"/>
+      <c r="B59" s="54"/>
+      <c r="C59" s="54"/>
+      <c r="D59" s="55"/>
+      <c r="E59" s="58"/>
+      <c r="F59" s="54"/>
       <c r="G59" s="19" t="s">
         <v>201</v>
       </c>
@@ -5389,17 +5389,17 @@
       <c r="A60" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B60" s="50" t="s">
+      <c r="B60" s="49" t="s">
         <v>249</v>
       </c>
-      <c r="C60" s="50" t="s">
+      <c r="C60" s="49" t="s">
         <v>250</v>
       </c>
-      <c r="D60" s="49" t="s">
+      <c r="D60" s="50" t="s">
         <v>86</v>
       </c>
       <c r="E60" s="15"/>
-      <c r="F60" s="50" t="s">
+      <c r="F60" s="49" t="s">
         <v>251</v>
       </c>
       <c r="G60" s="10" t="s">
@@ -5419,11 +5419,11 @@
       <c r="A61" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B61" s="50"/>
-      <c r="C61" s="50"/>
-      <c r="D61" s="49"/>
+      <c r="B61" s="49"/>
+      <c r="C61" s="49"/>
+      <c r="D61" s="50"/>
       <c r="E61" s="15"/>
-      <c r="F61" s="50"/>
+      <c r="F61" s="49"/>
       <c r="G61" s="10" t="s">
         <v>231</v>
       </c>
@@ -5438,19 +5438,19 @@
       <c r="A62" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B62" s="52" t="s">
+      <c r="B62" s="51" t="s">
         <v>266</v>
       </c>
-      <c r="C62" s="50" t="s">
+      <c r="C62" s="49" t="s">
         <v>213</v>
       </c>
-      <c r="D62" s="49" t="s">
+      <c r="D62" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="E62" s="51" t="s">
+      <c r="E62" s="56" t="s">
         <v>214</v>
       </c>
-      <c r="F62" s="50" t="s">
+      <c r="F62" s="49" t="s">
         <v>12</v>
       </c>
       <c r="G62" s="5" t="s">
@@ -5473,11 +5473,11 @@
       <c r="A63" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B63" s="52"/>
-      <c r="C63" s="50"/>
-      <c r="D63" s="49"/>
-      <c r="E63" s="51"/>
-      <c r="F63" s="50"/>
+      <c r="B63" s="51"/>
+      <c r="C63" s="49"/>
+      <c r="D63" s="50"/>
+      <c r="E63" s="56"/>
+      <c r="F63" s="49"/>
       <c r="G63" s="41" t="s">
         <v>190</v>
       </c>
@@ -5491,7 +5491,7 @@
       <c r="K63" s="41"/>
     </row>
     <row r="64" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="52"/>
+      <c r="B64" s="51"/>
       <c r="D64" s="36"/>
       <c r="E64" s="39"/>
       <c r="G64" s="41" t="s">
@@ -5573,12 +5573,12 @@
       <c r="A68" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B68" s="52" t="s">
+      <c r="B68" s="51" t="s">
         <v>230</v>
       </c>
       <c r="D68" s="12"/>
       <c r="E68" s="14"/>
-      <c r="F68" s="50" t="s">
+      <c r="F68" s="49" t="s">
         <v>232</v>
       </c>
       <c r="G68" s="5" t="s">
@@ -5595,10 +5595,10 @@
       <c r="A69" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B69" s="52"/>
+      <c r="B69" s="51"/>
       <c r="D69" s="12"/>
       <c r="E69" s="14"/>
-      <c r="F69" s="50"/>
+      <c r="F69" s="49"/>
       <c r="G69" s="5" t="s">
         <v>266</v>
       </c>
@@ -5610,7 +5610,7 @@
       </c>
     </row>
     <row r="70" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="52"/>
+      <c r="B70" s="51"/>
       <c r="D70" s="36"/>
       <c r="E70" s="39"/>
       <c r="G70" s="38" t="s">
@@ -5624,10 +5624,10 @@
       <c r="A71" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B71" s="52" t="s">
+      <c r="B71" s="51" t="s">
         <v>231</v>
       </c>
-      <c r="F71" s="50" t="s">
+      <c r="F71" s="49" t="s">
         <v>232</v>
       </c>
       <c r="G71" t="s">
@@ -5644,10 +5644,10 @@
       <c r="A72" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B72" s="52"/>
+      <c r="B72" s="51"/>
       <c r="D72" s="12"/>
       <c r="E72" s="14"/>
-      <c r="F72" s="50"/>
+      <c r="F72" s="49"/>
       <c r="G72" s="5" t="s">
         <v>266</v>
       </c>
@@ -5662,10 +5662,10 @@
       <c r="A73" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B73" s="52"/>
+      <c r="B73" s="51"/>
       <c r="D73" s="12"/>
       <c r="E73" s="14"/>
-      <c r="F73" s="50"/>
+      <c r="F73" s="49"/>
       <c r="G73" s="5" t="s">
         <v>261</v>
       </c>
@@ -5683,10 +5683,10 @@
       <c r="A74" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B74" s="52"/>
+      <c r="B74" s="51"/>
       <c r="D74" s="12"/>
       <c r="E74" s="15"/>
-      <c r="F74" s="50"/>
+      <c r="F74" s="49"/>
       <c r="G74" s="10" t="s">
         <v>249</v>
       </c>
@@ -5701,12 +5701,12 @@
       <c r="A75" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B75" s="58" t="s">
+      <c r="B75" s="57" t="s">
         <v>298</v>
       </c>
       <c r="D75" s="12"/>
       <c r="E75" s="14"/>
-      <c r="F75" s="50" t="s">
+      <c r="F75" s="49" t="s">
         <v>232</v>
       </c>
       <c r="G75" s="5" t="s">
@@ -5726,10 +5726,10 @@
       <c r="A76" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B76" s="58"/>
+      <c r="B76" s="57"/>
       <c r="D76" s="12"/>
       <c r="E76" s="14"/>
-      <c r="F76" s="50"/>
+      <c r="F76" s="49"/>
       <c r="G76" s="5" t="s">
         <v>231</v>
       </c>
@@ -5744,7 +5744,7 @@
       </c>
     </row>
     <row r="77" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="58"/>
+      <c r="B77" s="57"/>
       <c r="D77" s="24"/>
       <c r="E77" s="26"/>
       <c r="G77" s="25" t="s">
@@ -5761,19 +5761,19 @@
       <c r="A78" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B78" s="50" t="s">
+      <c r="B78" s="49" t="s">
         <v>190</v>
       </c>
-      <c r="C78" s="50" t="s">
+      <c r="C78" s="49" t="s">
         <v>234</v>
       </c>
-      <c r="D78" s="49" t="s">
+      <c r="D78" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="E78" s="51" t="s">
+      <c r="E78" s="56" t="s">
         <v>235</v>
       </c>
-      <c r="F78" s="50" t="s">
+      <c r="F78" s="49" t="s">
         <v>12</v>
       </c>
       <c r="G78" t="s">
@@ -5793,11 +5793,11 @@
       <c r="A79" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B79" s="50"/>
-      <c r="C79" s="50"/>
-      <c r="D79" s="49"/>
-      <c r="E79" s="51"/>
-      <c r="F79" s="50"/>
+      <c r="B79" s="49"/>
+      <c r="C79" s="49"/>
+      <c r="D79" s="50"/>
+      <c r="E79" s="56"/>
+      <c r="F79" s="49"/>
       <c r="G79" s="19" t="s">
         <v>205</v>
       </c>
@@ -5815,11 +5815,11 @@
       <c r="A80" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B80" s="50"/>
-      <c r="C80" s="50"/>
-      <c r="D80" s="49"/>
-      <c r="E80" s="51"/>
-      <c r="F80" s="50"/>
+      <c r="B80" s="49"/>
+      <c r="C80" s="49"/>
+      <c r="D80" s="50"/>
+      <c r="E80" s="56"/>
+      <c r="F80" s="49"/>
       <c r="G80" s="29" t="s">
         <v>198</v>
       </c>
@@ -5840,11 +5840,11 @@
       <c r="A81" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B81" s="50"/>
-      <c r="C81" s="50"/>
-      <c r="D81" s="49"/>
-      <c r="E81" s="51"/>
-      <c r="F81" s="50"/>
+      <c r="B81" s="49"/>
+      <c r="C81" s="49"/>
+      <c r="D81" s="50"/>
+      <c r="E81" s="56"/>
+      <c r="F81" s="49"/>
       <c r="G81" s="41" t="s">
         <v>266</v>
       </c>
@@ -5895,55 +5895,9 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="F78:F81"/>
-    <mergeCell ref="E78:E81"/>
-    <mergeCell ref="D78:D81"/>
-    <mergeCell ref="C78:C81"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="F23:F30"/>
-    <mergeCell ref="E23:E30"/>
-    <mergeCell ref="D23:D30"/>
-    <mergeCell ref="C23:C30"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="D49:D53"/>
-    <mergeCell ref="C49:C53"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="F49:F53"/>
-    <mergeCell ref="E49:E53"/>
-    <mergeCell ref="B23:B32"/>
+    <mergeCell ref="D54:D57"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="B54:B57"/>
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="B49:B53"/>
     <mergeCell ref="F44:F46"/>
@@ -5960,27 +5914,73 @@
     <mergeCell ref="B58:B59"/>
     <mergeCell ref="F54:F57"/>
     <mergeCell ref="E54:E57"/>
-    <mergeCell ref="D54:D57"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="D49:D53"/>
+    <mergeCell ref="C49:C53"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="F49:F53"/>
+    <mergeCell ref="E49:E53"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B23:B32"/>
+    <mergeCell ref="F23:F30"/>
+    <mergeCell ref="E23:E30"/>
+    <mergeCell ref="D23:D30"/>
+    <mergeCell ref="C23:C30"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="F78:F81"/>
+    <mergeCell ref="E78:E81"/>
+    <mergeCell ref="D78:D81"/>
+    <mergeCell ref="C78:C81"/>
+    <mergeCell ref="B78:B81"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6116,18 +6116,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49DDB8E0-B54A-48C7-9CD5-F6F83A84023D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FFAA9A4-7F5C-4158-AE1D-27A1D888CCD2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FFAA9A4-7F5C-4158-AE1D-27A1D888CCD2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49DDB8E0-B54A-48C7-9CD5-F6F83A84023D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>